<commit_message>
color added, folder selection added
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mac\Home\Documents\UiPath\PWC-Purchases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\UiPath\PWC-Purchases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD297B58-4B0E-475E-8CE6-B305A69D5878}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E064F8D1-5E0E-417C-A846-83B5B19BA059}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9218" xr2:uid="{CC834EF1-42AA-4737-8420-7857FAEAC985}"/>
   </bookViews>
@@ -89,12 +89,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,9 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -434,91 +448,91 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.9296875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" customWidth="1"/>
-    <col min="4" max="6" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.9296875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
+    <col min="5" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>4823006703</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>43537</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>43655</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>7736050003</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>43116</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>43486</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>105020580</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>5904082422</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>

</xml_diff>